<commit_message>
fixed bug in statistical dm
</commit_message>
<xml_diff>
--- a/data/cv_results_svm.xlsx
+++ b/data/cv_results_svm.xlsx
@@ -443,16 +443,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.004639307657877604</v>
+        <v>0.003323952356974284</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0004627233259380036</v>
+        <v>0.0004452725678422599</v>
       </c>
       <c r="D2" t="n">
-        <v>0.003657420476277669</v>
+        <v>0.001994689305623373</v>
       </c>
       <c r="E2" t="n">
-        <v>0.000470077941084057</v>
+        <v>8.104673248279548e-07</v>
       </c>
       <c r="F2" t="n">
         <v>1</v>
@@ -494,16 +494,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.005004485448201497</v>
+        <v>0.003667672475179037</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0007936475315081933</v>
+        <v>0.0009570149351590361</v>
       </c>
       <c r="D3" t="n">
-        <v>0.003409941991170248</v>
+        <v>0.002659320831298828</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0003943520335970096</v>
+        <v>0.000939415976526479</v>
       </c>
       <c r="F3" t="n">
         <v>1</v>
@@ -545,16 +545,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.005208253860473633</v>
+        <v>0.003346045811971029</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0005000962923220527</v>
+        <v>0.001229466340708883</v>
       </c>
       <c r="D4" t="n">
-        <v>0.00300137201944987</v>
+        <v>0.001662810643513997</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0007666301205233276</v>
+        <v>0.0004714277653650701</v>
       </c>
       <c r="F4" t="n">
         <v>1</v>
@@ -596,16 +596,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.005210558573404948</v>
+        <v>0.002304315567016602</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0009847936930681685</v>
+        <v>0.0004865479313779051</v>
       </c>
       <c r="D5" t="n">
-        <v>0.001752217610677083</v>
+        <v>0.001662492752075195</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0003560312623770807</v>
+        <v>0.0004924637568278591</v>
       </c>
       <c r="F5" t="n">
         <v>1</v>
@@ -647,16 +647,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.004994471867879231</v>
+        <v>0.002981265385945638</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0008256286873789565</v>
+        <v>1.439139168347066e-05</v>
       </c>
       <c r="D6" t="n">
-        <v>0.003659645716349284</v>
+        <v>0.002005418141682943</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0009417856253834899</v>
+        <v>2.93918528865542e-05</v>
       </c>
       <c r="F6" t="n">
         <v>10</v>
@@ -698,16 +698,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.004655122756958008</v>
+        <v>0.002327283223470052</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0004377662476140212</v>
+        <v>0.0004694598580568356</v>
       </c>
       <c r="D7" t="n">
-        <v>0.003655433654785156</v>
+        <v>0.001340389251708984</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0004713729263647648</v>
+        <v>0.0004860375447421871</v>
       </c>
       <c r="F7" t="n">
         <v>10</v>
@@ -749,16 +749,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.004868984222412109</v>
+        <v>0.004321177800496419</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0006750097784083211</v>
+        <v>0.001879861875499347</v>
       </c>
       <c r="D8" t="n">
-        <v>0.002161264419555664</v>
+        <v>0.002327521642049154</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0007324658269327509</v>
+        <v>0.0004708084360109519</v>
       </c>
       <c r="F8" t="n">
         <v>10</v>
@@ -800,16 +800,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.008595625559488932</v>
+        <v>0.002992788950602213</v>
       </c>
       <c r="C9" t="n">
-        <v>0.004413540092605458</v>
+        <v>0.001410964096548703</v>
       </c>
       <c r="D9" t="n">
-        <v>0.002043247222900391</v>
+        <v>0.003010272979736328</v>
       </c>
       <c r="E9" t="n">
-        <v>7.299996388338561e-05</v>
+        <v>0.001437713415015756</v>
       </c>
       <c r="F9" t="n">
         <v>10</v>
@@ -851,16 +851,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.004975398381551106</v>
+        <v>0.003342787424723307</v>
       </c>
       <c r="C10" t="n">
-        <v>0.001403041059607094</v>
+        <v>0.0004811230347141793</v>
       </c>
       <c r="D10" t="n">
-        <v>0.003668864568074544</v>
+        <v>0.002653121948242188</v>
       </c>
       <c r="E10" t="n">
-        <v>0.001254733088314233</v>
+        <v>0.0009279066708331331</v>
       </c>
       <c r="F10" t="n">
         <v>100</v>
@@ -902,16 +902,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.006332953770955403</v>
+        <v>0.003325541814168294</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0004806131161446417</v>
+        <v>0.000474858483440153</v>
       </c>
       <c r="D11" t="n">
-        <v>0.00341033935546875</v>
+        <v>0.001329501469930013</v>
       </c>
       <c r="E11" t="n">
-        <v>0.000422570863779735</v>
+        <v>0.000444239793616943</v>
       </c>
       <c r="F11" t="n">
         <v>100</v>
@@ -953,16 +953,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.006324132283528646</v>
+        <v>0.002660115559895833</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0004678033508640064</v>
+        <v>0.0004704916395046088</v>
       </c>
       <c r="D12" t="n">
-        <v>0.00329438845316569</v>
+        <v>0.00134126345316569</v>
       </c>
       <c r="E12" t="n">
-        <v>0.0004547378975671962</v>
+        <v>0.0004618466899366043</v>
       </c>
       <c r="F12" t="n">
         <v>100</v>
@@ -1004,16 +1004,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.005308628082275391</v>
+        <v>0.002671321233113607</v>
       </c>
       <c r="C13" t="n">
-        <v>0.0004355506577513702</v>
+        <v>0.0004785059628636676</v>
       </c>
       <c r="D13" t="n">
-        <v>0.003664573033650716</v>
+        <v>0.001972357432047526</v>
       </c>
       <c r="E13" t="n">
-        <v>0.0004641852922887119</v>
+        <v>0.0008025588762342157</v>
       </c>
       <c r="F13" t="n">
         <v>100</v>
@@ -1055,16 +1055,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>0.005732138951619466</v>
+        <v>0.002657492955525716</v>
       </c>
       <c r="C14" t="n">
-        <v>0.0005336591226334295</v>
+        <v>0.0009384700085535198</v>
       </c>
       <c r="D14" t="n">
-        <v>0.003259738286336263</v>
+        <v>0.002316554387410482</v>
       </c>
       <c r="E14" t="n">
-        <v>0.0009956370583991704</v>
+        <v>0.0004552983971299241</v>
       </c>
       <c r="F14" t="n">
         <v>1000</v>
@@ -1106,16 +1106,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.005330403645833333</v>
+        <v>0.004008769989013672</v>
       </c>
       <c r="C15" t="n">
-        <v>0.0004741092509242686</v>
+        <v>0.001434849717396358</v>
       </c>
       <c r="D15" t="n">
-        <v>0.00305477778116862</v>
+        <v>0.001972277959187826</v>
       </c>
       <c r="E15" t="n">
-        <v>0.0008046025343952935</v>
+        <v>0.001416918524317377</v>
       </c>
       <c r="F15" t="n">
         <v>1000</v>
@@ -1157,16 +1157,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0.006292819976806641</v>
+        <v>0.003325939178466797</v>
       </c>
       <c r="C16" t="n">
-        <v>0.0004572856330922091</v>
+        <v>0.001245026035683998</v>
       </c>
       <c r="D16" t="n">
-        <v>0.004011948903401692</v>
+        <v>0.002005736033121745</v>
       </c>
       <c r="E16" t="n">
-        <v>2.293642355776831e-05</v>
+        <v>0.0008270858453644146</v>
       </c>
       <c r="F16" t="n">
         <v>1000</v>
@@ -1208,16 +1208,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.005175908406575521</v>
+        <v>0.002326250076293945</v>
       </c>
       <c r="C17" t="n">
-        <v>0.0001320589775000805</v>
+        <v>0.0004703591919349732</v>
       </c>
       <c r="D17" t="n">
-        <v>0.002785444259643555</v>
+        <v>0.001651763916015625</v>
       </c>
       <c r="E17" t="n">
-        <v>0.0001456575571975936</v>
+        <v>0.0004627821924254846</v>
       </c>
       <c r="F17" t="n">
         <v>1000</v>

</xml_diff>